<commit_message>
Misc fixes and enhancements Updated some files to function properly (removed rows with headers, etc). Updated stats to include int and datetime Added Inferred_type column to summary
</commit_message>
<xml_diff>
--- a/Data/Avnet JP March 2020.xlsx
+++ b/Data/Avnet JP March 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrusp\Documents\SiTime Sales Data\Distrib_POS\Avnet Japan\2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JeffreyGeorge\PycharmProjects\SiTimeFileAnalysis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8834CFA7-8890-4C21-8E32-A7A8AC2BD963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEAB33A-A0DC-43DC-A1FA-2FB3F2886118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9890C5F-0A8C-4A8C-8FE9-3DC481C99C2D}"/>
+    <workbookView xWindow="-13770" yWindow="-19530" windowWidth="17280" windowHeight="15640" xr2:uid="{C9890C5F-0A8C-4A8C-8FE9-3DC481C99C2D}"/>
   </bookViews>
   <sheets>
     <sheet name="POS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
   <si>
     <t>Distributor</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>SIT8008BC-13-33E-27.000000E</t>
-  </si>
-  <si>
-    <t>Avnet Japan March 2020</t>
   </si>
   <si>
     <t>DATE</t>
@@ -478,68 +475,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30DE337-F3A1-4D87-9F5D-491600DDF22E}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.47265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.47265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="H2">
+        <v>250</v>
+      </c>
+      <c r="I2">
+        <v>0.45</v>
+      </c>
+      <c r="J2">
+        <v>0.55900000000000005</v>
       </c>
       <c r="K2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="M2">
+        <v>2020</v>
+      </c>
+      <c r="N2" s="1">
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -550,16 +577,16 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H3">
         <v>250</v>
       </c>
       <c r="I3">
-        <v>0.45</v>
+        <v>0.51100000000000001</v>
       </c>
       <c r="J3">
-        <v>0.55900000000000005</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="K3" t="s">
         <v>17</v>
@@ -574,7 +601,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -585,16 +612,16 @@
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H4">
         <v>250</v>
       </c>
       <c r="I4">
-        <v>0.51100000000000001</v>
+        <v>0.45</v>
       </c>
       <c r="J4">
-        <v>0.63400000000000001</v>
+        <v>0.55900000000000005</v>
       </c>
       <c r="K4" t="s">
         <v>17</v>
@@ -609,7 +636,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -620,16 +647,16 @@
         <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H5">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="I5">
         <v>0.45</v>
       </c>
       <c r="J5">
-        <v>0.55900000000000005</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="K5" t="s">
         <v>17</v>
@@ -644,7 +671,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -652,19 +679,19 @@
         <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H6">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="I6">
-        <v>0.45</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="J6">
-        <v>0.55500000000000005</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="K6" t="s">
         <v>17</v>
@@ -679,7 +706,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -687,19 +714,19 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H7">
-        <v>3000</v>
+        <v>250</v>
       </c>
       <c r="I7">
-        <v>0.35899999999999999</v>
+        <v>0.73199999999999998</v>
       </c>
       <c r="J7">
-        <v>0.45600000000000002</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="K7" t="s">
         <v>17</v>
@@ -714,7 +741,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -722,19 +749,19 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H8">
         <v>250</v>
       </c>
       <c r="I8">
-        <v>0.73199999999999998</v>
+        <v>0.51100000000000001</v>
       </c>
       <c r="J8">
-        <v>0.84799999999999998</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="K8" t="s">
         <v>17</v>
@@ -749,7 +776,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -757,19 +784,19 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H9">
-        <v>250</v>
+        <v>1000</v>
       </c>
       <c r="I9">
-        <v>0.51100000000000001</v>
+        <v>0.39</v>
       </c>
       <c r="J9">
-        <v>0.64800000000000002</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="K9" t="s">
         <v>17</v>
@@ -784,43 +811,8 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10">
-        <v>1000</v>
-      </c>
-      <c r="I10">
-        <v>0.39</v>
-      </c>
-      <c r="J10">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="K10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10">
-        <v>2020</v>
-      </c>
-      <c r="N10" s="1">
-        <v>43905</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="O11">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+      <c r="O10">
         <v>5750</v>
       </c>
     </row>

</xml_diff>